<commit_message>
updated test assets. new module WIP ismovementshorizontaldates. big update on SimulationContext.
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68E0077-2860-4E53-BF35-631F04A8EA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0399B43-4EFC-4F80-A8E1-B8326B66F294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="costi e ricavi simulazione" sheetId="1" r:id="rId1"/>
@@ -234,12 +234,6 @@
     <t>{intercompany:'aaa', financed:'xxx'} // financed viene scaricato per cassa</t>
   </si>
   <si>
-    <t>$$ mod GenericMovement.Set</t>
-  </si>
-  <si>
-    <t>$$ mod GenericMovement.Settings</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -1448,6 +1442,12 @@
   </si>
   <si>
     <t>no settings…</t>
+  </si>
+  <si>
+    <t>$$ mod GenericMovements.Settings</t>
+  </si>
+  <si>
+    <t>$$ mod GenericMovements.Set</t>
   </si>
 </sst>
 </file>
@@ -3297,7 +3297,9 @@
   </sheetPr>
   <dimension ref="A1:CM110"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3314,7 +3316,7 @@
   <sheetData>
     <row r="1" spans="1:91" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="3"/>
       <c r="E1" s="2"/>
@@ -3404,7 +3406,7 @@
     </row>
     <row r="3" spans="1:91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:91" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
@@ -3466,7 +3468,7 @@
     </row>
     <row r="6" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="28"/>
@@ -3516,7 +3518,7 @@
     </row>
     <row r="7" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="28"/>
@@ -3566,7 +3568,7 @@
     </row>
     <row r="8" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="28"/>
@@ -3616,7 +3618,7 @@
     </row>
     <row r="9" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="28"/>
@@ -3666,7 +3668,7 @@
     </row>
     <row r="10" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="25"/>
@@ -3716,7 +3718,7 @@
     </row>
     <row r="11" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="25"/>
@@ -3766,7 +3768,7 @@
     </row>
     <row r="12" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="25"/>
@@ -3816,7 +3818,7 @@
     </row>
     <row r="13" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="25"/>
@@ -4787,7 +4789,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" s="18">
         <v>29910.9</v>
@@ -4843,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C32" s="18">
         <v>37664.78</v>
@@ -9127,7 +9129,7 @@
   <dimension ref="A1:G187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9141,7 +9143,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -9149,23 +9151,23 @@
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>461</v>
       </c>
       <c r="B3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
         <v>65</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B5" s="47">
         <v>44926</v>
@@ -9177,7 +9179,7 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7"/>
       <c r="C7" s="46" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
@@ -9186,41 +9188,41 @@
     </row>
     <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="47"/>
       <c r="C9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="47"/>
       <c r="C10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="47"/>
       <c r="C11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="47"/>
       <c r="C12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="47"/>
       <c r="C13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -9242,7 +9244,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="30">
         <v>700924.19</v>
@@ -9259,7 +9261,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="30">
         <v>345442.02</v>
@@ -9273,7 +9275,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" s="30">
         <v>198668.46</v>
@@ -9287,7 +9289,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" s="30">
         <v>176465.34</v>
@@ -9301,35 +9303,35 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" s="30">
         <v>117999.24</v>
       </c>
       <c r="C19" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B20" s="30">
         <v>107617.42</v>
       </c>
       <c r="C20" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B21" s="30">
         <v>95233.2</v>
@@ -9338,12 +9340,12 @@
         <v>-1</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B22" s="30">
         <v>94237.68</v>
@@ -9357,7 +9359,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B23" s="30">
         <v>81829.119999999995</v>
@@ -9371,7 +9373,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B24" s="30">
         <v>61570.96</v>
@@ -9385,7 +9387,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B25" s="30">
         <v>43840</v>
@@ -9399,7 +9401,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B26" s="30">
         <v>39465.78</v>
@@ -9413,7 +9415,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B27" s="30">
         <v>30672</v>
@@ -9427,7 +9429,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B28" s="30">
         <v>25640</v>
@@ -9441,7 +9443,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B29" s="30">
         <v>21411</v>
@@ -9455,7 +9457,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30" s="30">
         <v>20909.71</v>
@@ -9469,7 +9471,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B31" s="30">
         <v>20659.48</v>
@@ -9483,7 +9485,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B32" s="30">
         <v>20000</v>
@@ -9497,7 +9499,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" s="30">
         <v>18217.2</v>
@@ -9511,7 +9513,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B34" s="30">
         <v>16826.16</v>
@@ -9525,7 +9527,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B35" s="30">
         <v>16440.96</v>
@@ -9539,7 +9541,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B36" s="30">
         <v>11000</v>
@@ -9553,7 +9555,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" s="30">
         <v>10701.84</v>
@@ -9567,7 +9569,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B38" s="30">
         <v>9760</v>
@@ -9578,7 +9580,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B39" s="30">
         <v>9496.99</v>
@@ -9592,7 +9594,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B40" s="30">
         <v>8026.32</v>
@@ -9603,7 +9605,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B41" s="30">
         <v>7799.21</v>
@@ -9617,7 +9619,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B42" s="30">
         <v>6459.82</v>
@@ -9631,7 +9633,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B43" s="30">
         <v>6173.2</v>
@@ -9645,7 +9647,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B44" s="30">
         <v>6087.59</v>
@@ -9656,7 +9658,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B45" s="30">
         <v>5717.25</v>
@@ -9667,7 +9669,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B46" s="30">
         <v>5634.55</v>
@@ -9678,7 +9680,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B47" s="30">
         <v>5537.35</v>
@@ -9692,7 +9694,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B48" s="30">
         <v>5413.14</v>
@@ -9706,7 +9708,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B49" s="30">
         <v>4944.91</v>
@@ -9720,7 +9722,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B50" s="30">
         <v>4701.28</v>
@@ -9731,7 +9733,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B51" s="30">
         <v>4650.6499999999996</v>
@@ -9745,7 +9747,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B52" s="30">
         <v>4640.88</v>
@@ -9759,7 +9761,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B53" s="30">
         <v>4323</v>
@@ -9773,7 +9775,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B54" s="30">
         <v>4076.19</v>
@@ -9784,7 +9786,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B55" s="30">
         <v>3776</v>
@@ -9795,7 +9797,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B56" s="30">
         <v>3658.61</v>
@@ -9806,7 +9808,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B57" s="30">
         <v>3313.48</v>
@@ -9817,7 +9819,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" s="30">
         <v>2937.94</v>
@@ -9828,7 +9830,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B59" s="30">
         <v>2906.82</v>
@@ -9839,7 +9841,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B60" s="30">
         <v>2867.7</v>
@@ -9850,7 +9852,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B61" s="30">
         <v>2554.1</v>
@@ -9861,7 +9863,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B62" s="30">
         <v>2549.1999999999998</v>
@@ -9872,7 +9874,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B63" s="30">
         <v>2491.7600000000002</v>
@@ -9883,7 +9885,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B64" s="30">
         <v>2460</v>
@@ -9894,7 +9896,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B65" s="30">
         <v>2440</v>
@@ -9905,7 +9907,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B66" s="30">
         <v>2414.29</v>
@@ -9916,7 +9918,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B67" s="30">
         <v>2379.36</v>
@@ -9927,7 +9929,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B68" s="30">
         <v>2249.9699999999998</v>
@@ -9938,7 +9940,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B69" s="30">
         <v>2221.5100000000002</v>
@@ -9949,7 +9951,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B70" s="30">
         <v>2038.1</v>
@@ -9960,7 +9962,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B71" s="30">
         <v>2038.1</v>
@@ -9971,7 +9973,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B72" s="30">
         <v>1906.7</v>
@@ -9982,7 +9984,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B73" s="30">
         <v>1859.5</v>
@@ -9993,7 +9995,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B74" s="30">
         <v>1785.96</v>
@@ -10004,7 +10006,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B75" s="30">
         <v>1680.9</v>
@@ -10015,7 +10017,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B76" s="30">
         <v>1652.27</v>
@@ -10026,7 +10028,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B77" s="30">
         <v>1500.6</v>
@@ -10037,7 +10039,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B78" s="30">
         <v>1439.73</v>
@@ -10048,7 +10050,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B79" s="30">
         <v>1429.22</v>
@@ -10059,7 +10061,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B80" s="30">
         <v>1327.96</v>
@@ -10070,7 +10072,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B81" s="30">
         <v>1295.7</v>
@@ -10081,7 +10083,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B82" s="30">
         <v>1243.17</v>
@@ -10092,7 +10094,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B83" s="30">
         <v>1190.6300000000001</v>
@@ -10103,7 +10105,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B84" s="30">
         <v>1145.5999999999999</v>
@@ -10114,7 +10116,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B85" s="30">
         <v>1144.68</v>
@@ -10125,7 +10127,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B86" s="30">
         <v>1033.06</v>
@@ -10136,7 +10138,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B87" s="30">
         <v>985.35</v>
@@ -10147,7 +10149,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B88" s="30">
         <v>983.11</v>
@@ -10158,7 +10160,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B89" s="30">
         <v>908.3</v>
@@ -10169,7 +10171,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B90" s="30">
         <v>903.5</v>
@@ -10180,7 +10182,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B91" s="30">
         <v>897</v>
@@ -10191,7 +10193,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B92" s="30">
         <v>878.4</v>
@@ -10202,7 +10204,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B93" s="30">
         <v>861.47</v>
@@ -10213,7 +10215,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B94" s="30">
         <v>857.97</v>
@@ -10224,7 +10226,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B95" s="30">
         <v>848.79</v>
@@ -10235,7 +10237,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B96" s="30">
         <v>840.46</v>
@@ -10246,7 +10248,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B97" s="30">
         <v>840</v>
@@ -10257,7 +10259,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B98" s="30">
         <v>834.24</v>
@@ -10268,7 +10270,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B99" s="30">
         <v>774.8</v>
@@ -10279,7 +10281,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B100" s="30">
         <v>725.4</v>
@@ -10290,7 +10292,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B101" s="30">
         <v>678.49</v>
@@ -10301,7 +10303,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B102" s="30">
         <v>667.37</v>
@@ -10312,7 +10314,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B103" s="30">
         <v>651.6</v>
@@ -10323,7 +10325,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B104" s="30">
         <v>601.89</v>
@@ -10334,7 +10336,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B105" s="30">
         <v>595</v>
@@ -10345,7 +10347,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B106" s="30">
         <v>578.07000000000005</v>
@@ -10356,7 +10358,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B107" s="30">
         <v>573</v>
@@ -10367,7 +10369,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B108" s="30">
         <v>563.70000000000005</v>
@@ -10378,7 +10380,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B109" s="30">
         <v>536.23</v>
@@ -10389,7 +10391,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B110" s="30">
         <v>521.77</v>
@@ -10400,7 +10402,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B111" s="30">
         <v>491.63</v>
@@ -10411,7 +10413,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B112" s="30">
         <v>491.25</v>
@@ -10422,7 +10424,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B113" s="30">
         <v>481.51</v>
@@ -10433,7 +10435,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B114" s="30">
         <v>474.36</v>
@@ -10444,7 +10446,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B115" s="30">
         <v>433.5</v>
@@ -10455,7 +10457,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B116" s="30">
         <v>425</v>
@@ -10466,7 +10468,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B117" s="30">
         <v>408.82</v>
@@ -10477,7 +10479,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B118" s="30">
         <v>392.35</v>
@@ -10488,7 +10490,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B119" s="30">
         <v>382.24</v>
@@ -10499,7 +10501,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B120" s="30">
         <v>373.02</v>
@@ -10510,7 +10512,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B121" s="30">
         <v>341.43</v>
@@ -10521,7 +10523,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B122" s="30">
         <v>312.56</v>
@@ -10532,7 +10534,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B123" s="30">
         <v>303.05</v>
@@ -10543,7 +10545,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B124" s="30">
         <v>296.98</v>
@@ -10554,7 +10556,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B125" s="30">
         <v>292.8</v>
@@ -10565,7 +10567,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B126" s="30">
         <v>292.8</v>
@@ -10576,7 +10578,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B127" s="30">
         <v>290.92</v>
@@ -10587,7 +10589,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B128" s="30">
         <v>278.89</v>
@@ -10598,7 +10600,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B129" s="30">
         <v>278.20999999999998</v>
@@ -10609,7 +10611,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B130" s="30">
         <v>275.23</v>
@@ -10620,7 +10622,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B131" s="30">
         <v>259.13</v>
@@ -10631,7 +10633,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B132" s="30">
         <v>254.37</v>
@@ -10642,7 +10644,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B133" s="30">
         <v>243.04</v>
@@ -10653,7 +10655,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B134" s="30">
         <v>231.24</v>
@@ -10664,7 +10666,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B135" s="30">
         <v>226.92</v>
@@ -10675,7 +10677,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B136" s="30">
         <v>214.49</v>
@@ -10686,7 +10688,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B137" s="30">
         <v>206.97</v>
@@ -10697,7 +10699,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B138" s="30">
         <v>190.31</v>
@@ -10708,7 +10710,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B139" s="30">
         <v>187.47</v>
@@ -10719,7 +10721,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B140" s="30">
         <v>179.97</v>
@@ -10730,7 +10732,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B141" s="30">
         <v>176.78</v>
@@ -10741,7 +10743,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B142" s="30">
         <v>172.9</v>
@@ -10752,7 +10754,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B143" s="30">
         <v>159.58000000000001</v>
@@ -10763,7 +10765,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B144" s="30">
         <v>136.58000000000001</v>
@@ -10774,7 +10776,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B145" s="30">
         <v>128.31</v>
@@ -10785,7 +10787,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B146" s="30">
         <v>120.38</v>
@@ -10796,7 +10798,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B147" s="30">
         <v>102.48</v>
@@ -10807,7 +10809,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B148" s="30">
         <v>96.94</v>
@@ -10818,7 +10820,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B149" s="30">
         <v>85</v>
@@ -10829,7 +10831,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B150" s="30">
         <v>76.8</v>
@@ -10840,7 +10842,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B151" s="30">
         <v>75.3</v>
@@ -10851,7 +10853,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B152" s="30">
         <v>70.5</v>
@@ -10862,7 +10864,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B153" s="30">
         <v>56</v>
@@ -10873,7 +10875,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B154" s="30">
         <v>55.24</v>
@@ -10884,7 +10886,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B155" s="30">
         <v>54.5</v>
@@ -10895,7 +10897,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B156" s="30">
         <v>51.24</v>
@@ -10906,7 +10908,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B157" s="30">
         <v>50</v>
@@ -10917,7 +10919,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B158" s="30">
         <v>48.17</v>
@@ -10928,7 +10930,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B159" s="30">
         <v>32.11</v>
@@ -10939,7 +10941,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B160" s="30">
         <v>21</v>
@@ -10950,7 +10952,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B161" s="30">
         <v>20</v>
@@ -10961,7 +10963,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B162" s="30">
         <v>18.82</v>
@@ -10972,7 +10974,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B163" s="30">
         <v>17</v>
@@ -10983,7 +10985,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B164" s="30">
         <v>15</v>
@@ -10994,7 +10996,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B165" s="30">
         <v>15</v>
@@ -11005,7 +11007,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B166" s="30">
         <v>14.5</v>
@@ -11016,7 +11018,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B167" s="30">
         <v>14</v>
@@ -11027,7 +11029,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B168" s="30">
         <v>14</v>
@@ -11038,7 +11040,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B169" s="30">
         <v>13.95</v>
@@ -11049,7 +11051,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B170" s="30">
         <v>8.36</v>
@@ -11060,7 +11062,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B171" s="30">
         <v>8</v>
@@ -11071,7 +11073,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B172" s="30">
         <v>0</v>
@@ -11082,7 +11084,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B173" s="30">
         <v>0</v>
@@ -11093,7 +11095,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B174" s="30">
         <v>0</v>
@@ -11104,7 +11106,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B175" s="30">
         <v>0</v>
@@ -11115,7 +11117,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B176" s="30">
         <v>0</v>
@@ -11126,7 +11128,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B177" s="30">
         <v>0</v>
@@ -11137,7 +11139,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B178" s="30">
         <v>-14.15</v>
@@ -11148,7 +11150,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B179" s="30">
         <v>-40.26</v>
@@ -11159,7 +11161,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B180" s="30">
         <v>-128.1</v>
@@ -11170,7 +11172,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B181" s="30">
         <v>-171.29</v>
@@ -11181,7 +11183,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B182" s="30">
         <v>-255.98</v>
@@ -11192,7 +11194,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B183" s="30">
         <v>-512.14</v>
@@ -11203,7 +11205,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B184" s="30">
         <v>-682.43</v>
@@ -11214,7 +11216,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B185" s="30">
         <v>-1975.07</v>
@@ -11230,7 +11232,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B187" s="45">
         <f>SUBTOTAL(109,CO__crediti2022[31/12/2022])</f>
@@ -11251,7 +11253,7 @@
   <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11265,28 +11267,28 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>461</v>
       </c>
       <c r="B3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B5" s="47">
         <v>44926</v>
@@ -11294,10 +11296,10 @@
     </row>
     <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="46"/>
@@ -11306,27 +11308,27 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -11348,7 +11350,7 @@
     </row>
     <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B15" s="38">
         <v>851474.64</v>
@@ -11357,18 +11359,18 @@
         <v>-1</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B16" s="38">
         <v>695155.84</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>43</v>
@@ -11376,7 +11378,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B17" s="38">
         <v>244488.74</v>
@@ -11390,13 +11392,13 @@
     </row>
     <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B18" s="38">
         <v>212666.6</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>45</v>
@@ -11404,13 +11406,13 @@
     </row>
     <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B19" s="38">
         <v>188072.09</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E19" s="42" t="s">
         <v>46</v>
@@ -11418,7 +11420,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B20" s="38">
         <v>155343.53</v>
@@ -11432,13 +11434,13 @@
     </row>
     <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B21" s="38">
         <v>145080.97</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E21" s="42" t="s">
         <v>47</v>
@@ -11446,13 +11448,13 @@
     </row>
     <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B22" s="38">
         <v>122466.16</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E22" s="42" t="s">
         <v>48</v>
@@ -11460,7 +11462,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B23" s="38">
         <v>97260.23</v>
@@ -11474,7 +11476,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B24" s="38">
         <v>81303.12</v>
@@ -11488,13 +11490,13 @@
     </row>
     <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B25" s="38">
         <v>61600</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>46</v>
@@ -11502,13 +11504,13 @@
     </row>
     <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B26" s="38">
         <v>60401.98</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E26" s="42" t="s">
         <v>46</v>
@@ -11516,13 +11518,13 @@
     </row>
     <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B27" s="38">
         <v>56309.13</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E27" s="42" t="s">
         <v>46</v>
@@ -11530,13 +11532,13 @@
     </row>
     <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B28" s="38">
         <v>55000</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E28" s="42" t="s">
         <v>46</v>
@@ -11544,7 +11546,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B29" s="38">
         <v>52175.74</v>
@@ -11558,13 +11560,13 @@
     </row>
     <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B30" s="38">
         <v>51146.03</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E30" s="42" t="s">
         <v>46</v>
@@ -11572,13 +11574,13 @@
     </row>
     <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B31" s="38">
         <v>49278.57</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E31" s="42" t="s">
         <v>46</v>
@@ -11586,13 +11588,13 @@
     </row>
     <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B32" s="38">
         <v>48819.42</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>46</v>
@@ -11600,13 +11602,13 @@
     </row>
     <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B33" s="38">
         <v>47580</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E33" s="42" t="s">
         <v>46</v>
@@ -11614,7 +11616,7 @@
     </row>
     <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B34" s="38">
         <v>46948.49</v>
@@ -11628,13 +11630,13 @@
     </row>
     <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B35" s="38">
         <v>45274.92</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>46</v>
@@ -11642,13 +11644,13 @@
     </row>
     <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B36" s="38">
         <v>42355.06</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E36" s="42" t="s">
         <v>46</v>
@@ -11656,13 +11658,13 @@
     </row>
     <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B37" s="38">
         <v>42284.11</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E37" s="42" t="s">
         <v>49</v>
@@ -11670,13 +11672,13 @@
     </row>
     <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B38" s="38">
         <v>41834.81</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>46</v>
@@ -11684,7 +11686,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B39" s="38">
         <v>40842.949999999997</v>
@@ -11698,13 +11700,13 @@
     </row>
     <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B40" s="38">
         <v>40543.78</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E40" s="42" t="s">
         <v>50</v>
@@ -11712,7 +11714,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B41" s="38">
         <v>38188</v>
@@ -11726,7 +11728,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B42" s="38">
         <v>35428.910000000003</v>
@@ -11740,13 +11742,13 @@
     </row>
     <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B43" s="38">
         <v>34116.22</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E43" s="42" t="s">
         <v>51</v>
@@ -11754,7 +11756,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B44" s="38">
         <v>34030.07</v>
@@ -11768,13 +11770,13 @@
     </row>
     <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B45" s="38">
         <v>32318.5</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E45" s="42" t="s">
         <v>53</v>
@@ -11782,13 +11784,13 @@
     </row>
     <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B46" s="38">
         <v>32108.45</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E46" s="42" t="s">
         <v>51</v>
@@ -11796,13 +11798,13 @@
     </row>
     <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B47" s="38">
         <v>30834.65</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E47" s="42" t="s">
         <v>46</v>
@@ -11810,7 +11812,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B48" s="38">
         <v>29960</v>
@@ -11824,13 +11826,13 @@
     </row>
     <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B49" s="38">
         <v>29682.45</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E49" s="42" t="s">
         <v>46</v>
@@ -11838,13 +11840,13 @@
     </row>
     <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B50" s="38">
         <v>25000</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E50" s="42" t="s">
         <v>46</v>
@@ -11852,13 +11854,13 @@
     </row>
     <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B51" s="38">
         <v>23714.76</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E51" s="42" t="s">
         <v>46</v>
@@ -11866,13 +11868,13 @@
     </row>
     <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B52" s="38">
         <v>23213.16</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E52" s="42" t="s">
         <v>46</v>
@@ -11880,7 +11882,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B53" s="38">
         <v>21177.98</v>
@@ -11891,7 +11893,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B54" s="38">
         <v>18671.919999999998</v>
@@ -11902,13 +11904,13 @@
     </row>
     <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B55" s="38">
         <v>18249.57</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E55" s="42" t="s">
         <v>54</v>
@@ -11916,7 +11918,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B56" s="38">
         <v>17882.759999999998</v>
@@ -11930,13 +11932,13 @@
     </row>
     <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B57" s="38">
         <v>17528.45</v>
       </c>
       <c r="C57" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E57" s="42" t="s">
         <v>54</v>
@@ -11944,7 +11946,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B58" s="38">
         <v>17160.95</v>
@@ -11958,13 +11960,13 @@
     </row>
     <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B59" s="38">
         <v>16367.84</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E59" s="42" t="s">
         <v>55</v>
@@ -11972,7 +11974,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B60" s="38">
         <v>15381.71</v>
@@ -11983,13 +11985,13 @@
     </row>
     <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B61" s="38">
         <v>15200.9</v>
       </c>
       <c r="C61" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E61" s="42" t="s">
         <v>54</v>
@@ -11997,7 +11999,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B62" s="38">
         <v>15159.5</v>
@@ -12011,7 +12013,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B63" s="38">
         <v>14981.6</v>
@@ -12025,13 +12027,13 @@
     </row>
     <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B64" s="38">
         <v>14875.7</v>
       </c>
       <c r="C64" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E64" s="42" t="s">
         <v>56</v>
@@ -12039,13 +12041,13 @@
     </row>
     <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B65" s="38">
         <v>14829.63</v>
       </c>
       <c r="C65" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E65" s="42" t="s">
         <v>56</v>
@@ -12053,13 +12055,13 @@
     </row>
     <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B66" s="38">
         <v>14740.49</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E66" s="42" t="s">
         <v>56</v>
@@ -12067,13 +12069,13 @@
     </row>
     <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B67" s="38">
         <v>14420.08</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E67" s="42" t="s">
         <v>56</v>
@@ -12081,13 +12083,13 @@
     </row>
     <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B68" s="38">
         <v>14233.58</v>
       </c>
       <c r="C68" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E68" s="42" t="s">
         <v>56</v>
@@ -12095,13 +12097,13 @@
     </row>
     <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B69" s="38">
         <v>14232.93</v>
       </c>
       <c r="C69" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E69" s="42" t="s">
         <v>56</v>
@@ -12109,13 +12111,13 @@
     </row>
     <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B70" s="38">
         <v>13750</v>
       </c>
       <c r="C70" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E70" s="42" t="s">
         <v>56</v>
@@ -12123,13 +12125,13 @@
     </row>
     <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B71" s="38">
         <v>13267.63</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E71" s="42" t="s">
         <v>56</v>
@@ -12137,7 +12139,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B72" s="38">
         <v>13202</v>
@@ -12148,13 +12150,13 @@
     </row>
     <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B73" s="38">
         <v>13123.71</v>
       </c>
       <c r="C73" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E73" s="42" t="s">
         <v>56</v>
@@ -12162,7 +12164,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B74" s="38">
         <v>13084.51</v>
@@ -12173,13 +12175,13 @@
     </row>
     <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B75" s="38">
         <v>11722.92</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E75" s="42" t="s">
         <v>56</v>
@@ -12187,13 +12189,13 @@
     </row>
     <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B76" s="38">
         <v>11714.56</v>
       </c>
       <c r="C76" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E76" s="42" t="s">
         <v>56</v>
@@ -12201,13 +12203,13 @@
     </row>
     <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B77" s="38">
         <v>11680.8</v>
       </c>
       <c r="C77" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E77" s="42" t="s">
         <v>56</v>
@@ -12215,7 +12217,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B78" s="38">
         <v>11508.38</v>
@@ -12229,7 +12231,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B79" s="38">
         <v>11316.23</v>
@@ -12240,7 +12242,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B80" s="38">
         <v>11122.71</v>
@@ -12251,13 +12253,13 @@
     </row>
     <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B81" s="38">
         <v>10787.57</v>
       </c>
       <c r="C81" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E81" s="42" t="s">
         <v>56</v>
@@ -12265,7 +12267,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B82" s="38">
         <v>10505.28</v>
@@ -12276,13 +12278,13 @@
     </row>
     <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B83" s="38">
         <v>10463.709999999999</v>
       </c>
       <c r="C83" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E83" s="42" t="s">
         <v>56</v>
@@ -12290,7 +12292,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B84" s="38">
         <v>10370</v>
@@ -12304,13 +12306,13 @@
     </row>
     <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B85" s="38">
         <v>9961.4500000000007</v>
       </c>
       <c r="C85" s="38" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E85" s="42" t="s">
         <v>57</v>
@@ -12318,7 +12320,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B86" s="38">
         <v>9754.69</v>
@@ -12329,7 +12331,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B87" s="38">
         <v>9563.2900000000009</v>
@@ -12343,7 +12345,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B88" s="38">
         <v>9360.4500000000007</v>
@@ -12357,13 +12359,13 @@
     </row>
     <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B89" s="38">
         <v>9358.25</v>
       </c>
       <c r="C89" s="38" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E89" s="42" t="s">
         <v>57</v>
@@ -12371,13 +12373,13 @@
     </row>
     <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B90" s="38">
         <v>8637.9699999999993</v>
       </c>
       <c r="C90" s="38" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E90" s="42" t="s">
         <v>57</v>
@@ -12385,7 +12387,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B91" s="38">
         <v>8408.93</v>
@@ -12396,7 +12398,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B92" s="38">
         <v>7933.17</v>
@@ -12407,7 +12409,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B93" s="38">
         <v>7924.8</v>
@@ -12421,13 +12423,13 @@
     </row>
     <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B94" s="38">
         <v>7735.25</v>
       </c>
       <c r="C94" s="38" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E94" s="42" t="s">
         <v>57</v>
@@ -12435,13 +12437,13 @@
     </row>
     <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B95" s="38">
         <v>7016.45</v>
       </c>
       <c r="C95" s="38" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E95" s="42" t="s">
         <v>57</v>
@@ -12449,7 +12451,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B96" s="38">
         <v>6832</v>
@@ -12463,7 +12465,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B97" s="38">
         <v>6758.88</v>
@@ -12474,7 +12476,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B98" s="38">
         <v>6093.36</v>
@@ -12488,7 +12490,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B99" s="38">
         <v>5795</v>
@@ -12502,7 +12504,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B100" s="38">
         <v>5764</v>
@@ -12516,7 +12518,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B101" s="38">
         <v>5502.35</v>
@@ -12530,13 +12532,13 @@
     </row>
     <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B102" s="38">
         <v>5407.75</v>
       </c>
       <c r="C102" s="38" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E102" s="42" t="s">
         <v>58</v>
@@ -12544,7 +12546,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B103" s="38">
         <v>5342.38</v>
@@ -12558,13 +12560,13 @@
     </row>
     <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B104" s="38">
         <v>5254.37</v>
       </c>
       <c r="C104" s="38" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E104" s="42" t="s">
         <v>58</v>
@@ -12572,13 +12574,13 @@
     </row>
     <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B105" s="38">
         <v>5211.95</v>
       </c>
       <c r="C105" s="38" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E105" s="42" t="s">
         <v>58</v>
@@ -12586,7 +12588,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B106" s="38">
         <v>5160</v>
@@ -12600,7 +12602,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B107" s="38">
         <v>5032.6000000000004</v>
@@ -12611,13 +12613,13 @@
     </row>
     <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B108" s="38">
         <v>4772.8999999999996</v>
       </c>
       <c r="C108" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E108" s="42" t="s">
         <v>59</v>
@@ -12625,7 +12627,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B109" s="38">
         <v>4538.87</v>
@@ -12636,7 +12638,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B110" s="38">
         <v>4454.6000000000004</v>
@@ -12650,13 +12652,13 @@
     </row>
     <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B111" s="38">
         <v>4266.5</v>
       </c>
       <c r="C111" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E111" s="42" t="s">
         <v>59</v>
@@ -12664,7 +12666,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B112" s="38">
         <v>4254.51</v>
@@ -12675,7 +12677,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B113" s="38">
         <v>4027.16</v>
@@ -12686,13 +12688,13 @@
     </row>
     <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B114" s="38">
         <v>3828</v>
       </c>
       <c r="C114" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E114" s="42" t="s">
         <v>59</v>
@@ -12700,7 +12702,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B115" s="38">
         <v>3733.2</v>
@@ -12711,13 +12713,13 @@
     </row>
     <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B116" s="38">
         <v>3614.27</v>
       </c>
       <c r="C116" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E116" s="42" t="s">
         <v>59</v>
@@ -12725,7 +12727,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B117" s="38">
         <v>3524.71</v>
@@ -12736,13 +12738,13 @@
     </row>
     <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B118" s="38">
         <v>3503.5</v>
       </c>
       <c r="C118" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E118" s="42" t="s">
         <v>59</v>
@@ -12750,13 +12752,13 @@
     </row>
     <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B119" s="38">
         <v>3409.48</v>
       </c>
       <c r="C119" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E119" s="42" t="s">
         <v>59</v>
@@ -12764,7 +12766,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B120" s="38">
         <v>3390.99</v>
@@ -12775,7 +12777,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B121" s="38">
         <v>3385.5</v>
@@ -12789,7 +12791,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B122" s="38">
         <v>3355</v>
@@ -12800,7 +12802,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B123" s="38">
         <v>3339.6</v>
@@ -12811,13 +12813,13 @@
     </row>
     <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B124" s="38">
         <v>3269.64</v>
       </c>
       <c r="C124" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E124" s="42" t="s">
         <v>59</v>
@@ -12825,13 +12827,13 @@
     </row>
     <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B125" s="38">
         <v>3040.8</v>
       </c>
       <c r="C125" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E125" s="42" t="s">
         <v>59</v>
@@ -12839,7 +12841,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B126" s="38">
         <v>2869.7</v>
@@ -12850,13 +12852,13 @@
     </row>
     <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B127" s="38">
         <v>2669.85</v>
       </c>
       <c r="C127" s="38" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E127" s="42" t="s">
         <v>60</v>
@@ -12864,13 +12866,13 @@
     </row>
     <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B128" s="38">
         <v>2562</v>
       </c>
       <c r="C128" s="38" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E128" s="42" t="s">
         <v>60</v>
@@ -12878,7 +12880,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B129" s="38">
         <v>2519.91</v>
@@ -12889,7 +12891,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B130" s="38">
         <v>2501</v>
@@ -12900,7 +12902,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B131" s="38">
         <v>2350.4</v>
@@ -12911,7 +12913,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B132" s="38">
         <v>2217.96</v>
@@ -12922,7 +12924,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B133" s="38">
         <v>2086.1999999999998</v>
@@ -12936,7 +12938,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B134" s="38">
         <v>2080</v>
@@ -12950,7 +12952,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B135" s="38">
         <v>2067.0100000000002</v>
@@ -12961,7 +12963,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B136" s="38">
         <v>2059.36</v>
@@ -12972,7 +12974,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B137" s="38">
         <v>2000</v>
@@ -12983,7 +12985,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B138" s="38">
         <v>1963.25</v>
@@ -12994,7 +12996,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B139" s="38">
         <v>1952</v>
@@ -13005,7 +13007,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B140" s="38">
         <v>1952</v>
@@ -13016,7 +13018,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B141" s="38">
         <v>1769</v>
@@ -13027,7 +13029,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B142" s="38">
         <v>1732</v>
@@ -13038,7 +13040,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B143" s="38">
         <v>1400.56</v>
@@ -13049,7 +13051,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B144" s="38">
         <v>1291.68</v>
@@ -13060,7 +13062,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B145" s="38">
         <v>1105.5999999999999</v>
@@ -13071,7 +13073,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B146" s="38">
         <v>1098</v>
@@ -13082,7 +13084,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B147" s="38">
         <v>1098</v>
@@ -13093,7 +13095,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B148" s="38">
         <v>1083.8499999999999</v>
@@ -13104,7 +13106,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B149" s="38">
         <v>1080</v>
@@ -13115,7 +13117,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B150" s="38">
         <v>1012.6</v>
@@ -13126,7 +13128,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B151" s="38">
         <v>980.98</v>
@@ -13137,7 +13139,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B152" s="38">
         <v>933.3</v>
@@ -13148,7 +13150,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B153" s="38">
         <v>915</v>
@@ -13159,7 +13161,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B154" s="38">
         <v>854</v>
@@ -13170,7 +13172,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B155" s="38">
         <v>829.65</v>
@@ -13181,7 +13183,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B156" s="38">
         <v>805.75</v>
@@ -13192,7 +13194,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B157" s="38">
         <v>788</v>
@@ -13203,7 +13205,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B158" s="38">
         <v>750.4</v>
@@ -13214,7 +13216,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B159" s="38">
         <v>748.8</v>
@@ -13225,7 +13227,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B160" s="38">
         <v>708</v>
@@ -13236,7 +13238,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B161" s="38">
         <v>678</v>
@@ -13247,7 +13249,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B162" s="38">
         <v>613.14</v>
@@ -13258,7 +13260,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B163" s="38">
         <v>585.6</v>
@@ -13269,7 +13271,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B164" s="38">
         <v>582.12</v>
@@ -13280,7 +13282,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B165" s="38">
         <v>492.8</v>
@@ -13291,7 +13293,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B166" s="38">
         <v>491.05</v>
@@ -13302,7 +13304,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B167" s="38">
         <v>488</v>
@@ -13313,7 +13315,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B168" s="38">
         <v>467.5</v>
@@ -13324,7 +13326,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B169" s="38">
         <v>457.5</v>
@@ -13335,7 +13337,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B170" s="38">
         <v>414.8</v>
@@ -13346,7 +13348,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B171" s="38">
         <v>411.4</v>
@@ -13357,7 +13359,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B172" s="38">
         <v>399.9</v>
@@ -13368,7 +13370,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B173" s="38">
         <v>374.7</v>
@@ -13379,7 +13381,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B174" s="38">
         <v>353.12</v>
@@ -13390,7 +13392,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B175" s="38">
         <v>341.6</v>
@@ -13401,7 +13403,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B176" s="38">
         <v>292.8</v>
@@ -13412,7 +13414,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B177" s="38">
         <v>288.64999999999998</v>
@@ -13423,7 +13425,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B178" s="38">
         <v>205.7</v>
@@ -13434,7 +13436,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B179" s="38">
         <v>200.08</v>
@@ -13445,7 +13447,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B180" s="38">
         <v>188.8</v>
@@ -13456,7 +13458,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B181" s="38">
         <v>158.4</v>
@@ -13467,7 +13469,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B182" s="38">
         <v>147.62</v>
@@ -13478,7 +13480,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B183" s="38">
         <v>144</v>
@@ -13489,7 +13491,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B184" s="38">
         <v>128.1</v>
@@ -13500,7 +13502,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B185" s="38">
         <v>123</v>
@@ -13511,7 +13513,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B186" s="38">
         <v>87.65</v>
@@ -13522,7 +13524,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B187" s="38">
         <v>84.91</v>
@@ -13533,7 +13535,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B188" s="38">
         <v>70</v>
@@ -13544,7 +13546,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B189" s="38">
         <v>69.599999999999994</v>
@@ -13555,7 +13557,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B190" s="38">
         <v>48.8</v>
@@ -13566,7 +13568,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B191" s="38">
         <v>47.58</v>
@@ -13577,7 +13579,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B192" s="38">
         <v>46.34</v>
@@ -13588,7 +13590,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B193" s="38">
         <v>30.18</v>
@@ -13599,7 +13601,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B194" s="38">
         <v>11.97</v>
@@ -13610,7 +13612,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B195" s="38">
         <v>0</v>
@@ -13621,7 +13623,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B196" s="38">
         <v>0</v>
@@ -13632,7 +13634,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B197" s="38">
         <v>-42.8</v>
@@ -13643,7 +13645,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B198" s="38">
         <v>-44.01</v>
@@ -13654,7 +13656,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B199" s="38">
         <v>-46.5</v>
@@ -13665,7 +13667,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B200" s="38">
         <v>-555.5</v>
@@ -13676,7 +13678,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B201" s="38">
         <v>-1740</v>
@@ -13687,7 +13689,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B202" s="45">
         <f>SUBTOTAL(109,CO__debiti2022[31/12/2022])</f>
@@ -13712,7 +13714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4483405-5FFC-4EDD-902E-75E3FB56B872}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -13722,7 +13724,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simplified settings module. implementing genericmovements.js. renaming utils file. improved sanitization utils
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B00222A-3054-4CB6-97C1-8029DD8FF01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3910EE98-18F5-4750-9FBB-BCAA36A0F9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>31/12/2022</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>BBB</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>opposite type</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
 </sst>
 </file>
@@ -302,10 +314,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A14:E16" totalsRowShown="0" headerRowBorderDxfId="5">
-  <autoFilter ref="A14:E16" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:B16">
-    <sortCondition descending="1" ref="B14:B16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A16:E18" totalsRowShown="0" headerRowBorderDxfId="5">
+  <autoFilter ref="A16:E18" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:B18">
+    <sortCondition descending="1" ref="B16:B18"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="Nominativo"/>
@@ -313,6 +325,17 @@
     <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}" name="Table5" displayName="Table5" ref="A4:B7" totalsRowShown="0">
+  <autoFilter ref="A4:B7" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2C543E85-0E79-4148-B6BE-1D8782461A75}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{4A4F48B5-D66B-4359-BE1C-810A473D05EC}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -615,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D13926F-0BD1-460D-BBDD-36F9AE527C93}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,114 +669,131 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B6" s="11">
         <v>44926</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B6"/>
-    </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B7"/>
-      <c r="C7" s="10" t="s">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9"/>
+      <c r="C9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8"/>
-      <c r="C8" t="s">
+      <c r="B10"/>
+      <c r="C10" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="11"/>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="11"/>
-      <c r="C10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="11"/>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="11"/>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
       <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="11"/>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="11"/>
+      <c r="C15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B17" s="3">
         <v>700924.19</v>
       </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B18" s="3">
         <v>345442.02</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E18" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated modules and test data
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB99DC9-FD2E-4B93-8F2D-6F5F29810978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDEF452-C2F4-4CB4-8763-A87B8378403A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="crediti a inizi 2023" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Nominativo</t>
   </si>
@@ -54,9 +54,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>TradeReceivableCredits</t>
-  </si>
-  <si>
     <t>$$ CLIENTI DA INCASSARE</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>escludi dalla simulazione righe dove "simulation input" = nullOrWhitespace; se per errore nella riga di totale c'è scritto qualcosa anche sulla riga di "simulation input" allora verrà presa, ma è inevitabile.</t>
   </si>
   <si>
-    <t>value column</t>
-  </si>
-  <si>
     <t>// {start:'2024-06-01', np:2, [npy:2]}  // piano francese, senza interessi</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>no settings…</t>
   </si>
   <si>
-    <t>$$ mod GenericMovements.Settings</t>
-  </si>
-  <si>
     <t>AAA</t>
   </si>
   <si>
@@ -108,19 +99,25 @@
     <t>Value</t>
   </si>
   <si>
-    <t>opposite type</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>2022-12-31</t>
-  </si>
-  <si>
     <t>mamma</t>
   </si>
   <si>
     <t>gino</t>
+  </si>
+  <si>
+    <t>#2022-12-31</t>
+  </si>
+  <si>
+    <t>vs type</t>
+  </si>
+  <si>
+    <t>BS_CREDIT__TRADERECEIVABLECREDITS</t>
+  </si>
+  <si>
+    <t>Bs_Cash__BankAccount_FinancialAccount</t>
+  </si>
+  <si>
+    <t>$$ mod GenericMovementsH.Settings</t>
   </si>
 </sst>
 </file>
@@ -229,7 +226,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -246,7 +243,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
@@ -257,7 +253,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -272,6 +267,18 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -290,17 +297,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -323,27 +319,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A16:E18" totalsRowShown="0" headerRowBorderDxfId="5">
-  <autoFilter ref="A16:E18" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:B18">
-    <sortCondition descending="1" ref="B16:B18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A15:E17" totalsRowShown="0" headerRowBorderDxfId="5">
+  <autoFilter ref="A15:E17" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:B17">
+    <sortCondition descending="1" ref="B15:B17"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="Nominativo"/>
-    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="2022-12-31" dataDxfId="2" totalsRowDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="0">
-      <calculatedColumnFormula>CO__crediti2022[[#This Row],[2022-12-31]]+2</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="2">
+      <calculatedColumnFormula>CO__crediti2022[[#This Row],['#2022-12-31]]+2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}" name="Table5" displayName="Table5" ref="A4:B7" totalsRowShown="0">
-  <autoFilter ref="A4:B7" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}" name="Table5" displayName="Table5" ref="A4:B6" totalsRowShown="0">
+  <autoFilter ref="A4:B6" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2C543E85-0E79-4148-B6BE-1D8782461A75}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4A4F48B5-D66B-4359-BE1C-810A473D05EC}" name="Value"/>
@@ -649,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D13926F-0BD1-460D-BBDD-36F9AE527C93}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -666,7 +662,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -674,18 +670,18 @@
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -693,126 +689,118 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
+      <c r="B7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B9"/>
-      <c r="C9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="10"/>
+      <c r="C10" t="s">
         <v>7</v>
-      </c>
-      <c r="B10"/>
-      <c r="C10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="10"/>
-      <c r="C15" t="s">
-        <v>15</v>
+      <c r="A15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
-        <v>100</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>26</v>
+        <v>150</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3">
-        <v>150</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="7"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" s="11"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="11"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="11"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -838,7 +826,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved genericmovementsh and other sanitization code
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDEF452-C2F4-4CB4-8763-A87B8378403A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EBBC16-1E03-40BE-8DC2-34C9545A35CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="crediti a inizi 2023" sheetId="2" r:id="rId1"/>
@@ -648,7 +648,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
new search method searchDateKeys in serch_utils. new checks in date_utils.
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EBBC16-1E03-40BE-8DC2-34C9545A35CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EBEB64-44BF-4259-A1BC-CF288CE9CFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Nominativo</t>
   </si>
@@ -129,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +176,12 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,7 +257,49 @@
     <cellStyle name="Comma 2 3" xfId="1" xr:uid="{D614F647-4E31-4F6F-A208-E19F25DAA59C}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -319,19 +367,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A15:E17" totalsRowShown="0" headerRowBorderDxfId="5">
-  <autoFilter ref="A15:E17" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A15:G17" totalsRowShown="0" headerRowBorderDxfId="9">
+  <autoFilter ref="A15:G17" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:B17">
     <sortCondition descending="1" ref="B15:B17"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="Nominativo"/>
-    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{A73DD4B2-FC57-4525-BC32-8602D7809823}" name="type" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{42E5DFF3-D73C-42FC-942C-4723FDD32704}" name="vs type" dataDxfId="2" totalsRowDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{703624DF-A066-447E-A078-0CAB43E2FA43}" name="simulation input" dataDxfId="6">
       <calculatedColumnFormula>CO__crediti2022[[#This Row],['#2022-12-31]]+2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{C484BE29-51EA-41D6-A5A0-246759D70030}" name="vs // name of related SimObjects" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -645,164 +695,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D13926F-0BD1-460D-BBDD-36F9AE527C93}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="68.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.1796875" customWidth="1"/>
-    <col min="5" max="5" width="49.08984375" customWidth="1"/>
+    <col min="2" max="4" width="15.54296875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="68.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.1796875" customWidth="1"/>
+    <col min="7" max="7" width="49.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C4"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C5"/>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C6"/>
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C7"/>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9"/>
-      <c r="C9" t="s">
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
-      <c r="C10" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
-      <c r="C11" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
-      <c r="C12" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
-      <c r="C13" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
-      <c r="C14" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3">
         <v>100</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3">
         <v>150</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G17" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B20" s="11"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
update modules, agenda, documents, test
</commit_message>
<xml_diff>
--- a/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
+++ b/tests/_end_to_end_tests/main-treasury-temp/user_data__no_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB717820-FD67-4685-8DC2-8ECA3B894EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA3DE55-70EA-4F4C-895E-2E6D533ABE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Nominativo</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>$$ mod GenericMovements.Settings</t>
+  </si>
+  <si>
+    <t>amount delta value</t>
   </si>
 </sst>
 </file>
@@ -367,10 +370,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A15:G17" totalsRowShown="0" headerRowBorderDxfId="9">
-  <autoFilter ref="A15:G17" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:B17">
-    <sortCondition descending="1" ref="B15:B17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A16:G18" totalsRowShown="0" headerRowBorderDxfId="9">
+  <autoFilter ref="A16:G18" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:B18">
+    <sortCondition descending="1" ref="B16:B18"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="Nominativo"/>
@@ -388,8 +391,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}" name="Table5" displayName="Table5" ref="A4:B6" totalsRowShown="0">
-  <autoFilter ref="A4:B6" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}" name="Table5" displayName="Table5" ref="A4:B7" totalsRowShown="0">
+  <autoFilter ref="A4:B7" xr:uid="{6272B443-DA45-4985-B709-05C8C4734883}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2C543E85-0E79-4148-B6BE-1D8782461A75}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4A4F48B5-D66B-4359-BE1C-810A473D05EC}" name="Value"/>
@@ -695,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D13926F-0BD1-460D-BBDD-36F9AE527C93}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -738,28 +741,33 @@
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
+    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B7"/>
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
       <c r="C7"/>
       <c r="D7"/>
     </row>
@@ -767,31 +775,28 @@
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
-      <c r="E8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
-      <c r="E9" t="s">
+      <c r="E9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -799,7 +804,7 @@
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -807,7 +812,7 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -815,7 +820,7 @@
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -823,70 +828,78 @@
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>100</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>100</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B18" s="3">
         <v>150</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>